<commit_message>
Get daily reddit data: Tue Jul  8 08:13:42 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_13.xlsx
+++ b/data/collected_data/2025_07_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C510"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3559 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1luif3q</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>New nails ^^ What can i improve</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nreanzlyrlbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1luia9u</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>I've never gotten acrylics before, what should I expect? Should I even get them?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1luia9u/ive_never_gotten_acrylics_before_what_should_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1luhmvg</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>ડꪀꪖⅈꪶꫀᦔ ⅈ𝕥 ! 🐌</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/680ok20hilbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1lufesc</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Freestyle w/ New Tech</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lufesc</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1luhd7d</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Fresh set🫧♥️</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vg44l1qeflbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1luh8um</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1luh8um</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1lugvkq</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Me and my friend got our rave nails done, what do you think</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jz7migft9lbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1lugq8h</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>pink summer glory by my nail tech</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/059mxj278lbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1lugdxp</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Need help brainstorming nail ideas based on this little guy!</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lugdxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1lugajs</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Toesss</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lugajs</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1lug4lv</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Beach vacay nails 🐚 🌊🧜‍♀️🌟</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lug4lv</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1lug4i8</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Beach vacay nails 🐚 🌊🧜‍♀️🌟</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lug4i8</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1lug434</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Finger Scales</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lug434</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1lufqxd</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>4mnth progress trying to build my own Press on brand. Any advice?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lufqxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1lufo93</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Press On Nails</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jtefhc5ywkbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1lua5og</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Raised sidewalls</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjs7znusjjbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1ludjex</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>can you help me decide the best nail shape for my hands based on these photos?</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ludjex</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1luephp</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>It's an inspiration, what do you think, yes or no? I like them🥹</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9iw1o3sjnkbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1lucrkq</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Help with nail!!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsjfflm46kbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1luex3y</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>What do you think of this colour for summer?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z09nf2hkpkbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1luevg7</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Going to the store. What to buy to remove these monstrosities??</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1luevg7</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1luelrr</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>finished these vacation nails today !</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1luelrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1lue67d</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>what is a good but cheapish gel polish brand or bundle to get started with?</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lue67d/what_is_a_good_but_cheapish_gel_polish_brand_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1lue1rn</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Did my birthday nails 😅</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v398htdfhkbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1ludkvl</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Red violet</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zyskuf9dkbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1ludi3h</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Press ons &amp; polish</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27h25gclckbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1lucx4i</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Love this new set</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lucx4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1lucncj</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>My young friends first time doing nails on someone</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mn38xru45kbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1lua9nw</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Idk if counts as a manicure, because they're just Kiss press-ons and a couple of random charms I found, but they look gorgeous and make me feel like a spoiled princess, so here's some French tip inspo, I guess? XD</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80ky9xkujjbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1luchec</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>I think red is the winning color</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzco9o8g3kbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1lua6rc</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>For me, by me🫶</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lua6rc</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1luceol</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>The temptation to just get a top coat.</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3jivckz2kbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1luc7n0</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Summer flowers + French</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1luc7n0</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1lubzr2</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Lemon set. Do you like them? 😍</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lubzr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1luboy8</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Summerween nails for a friend of mine</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ylhdalxnwjbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1lubeva</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>After many attempts of going for the perfect French manicure I finally feel like I got one at a salon</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rkops75fujbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1luatwa</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Just got dip nails removed</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1luatwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1lua5u9</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Is this good work? I had an appointment with my usual person but they had someone new do them and it was his first day!</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lua5u9</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1lua44e</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>I got my nails done today… and I hate them</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lua44e</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1lu9ts4</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Moody summer tortie</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjg58z72hjbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1lu9dk5</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Press on nail case storage ideas?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lu9dk5/press_on_nail_case_storage_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1lu926g</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Press on Nails [Help]</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lu926g/press_on_nails_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1lu88m9</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Natural nails. Used to keep them longer but can’t because of job.</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/na10ssrm4jbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1lu7xsz</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Anyone else fall out of love of doing their nails?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lu7xsz/anyone_else_fall_out_of_love_of_doing_their_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1lu7syt</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Nail tech school questions..</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qysivfwc1jbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1lu7qzw</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Can’t decide if I like them or not</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu7qzw</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1lu7m76</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Summer nails 🫧🌸</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu7m76</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1lu7d71</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Help with my nails</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mjw9zvb5yibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1lu76qo</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>my nails😍 vs my workspace after finishing😱</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu76qo</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1lu72mp</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Nude cateye can’t be beat💖</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uiflthpyvibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1lu70k7</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>I think they’re cute 💗</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu70k7</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1lu6xcn</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>🐮🐄</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2w16siwuibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1lu6f5h</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Is this considered lifting and how quickly should I take it off?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu6f5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1lu6clz</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Abstract DIY</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu6clz</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1lu62wt</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Brown circle in middle of nail</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79ou66wuoibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1lu63nu</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>got a twin peaks set done today 💙 🥀</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu63nu</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1lu5qsk</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Thought I should repost because this color is bomb</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/muds73xkmibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1lu5kjn</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>First half of 2025 in nails</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu5kjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1lu5k7n</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Purple Today Design</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05w07hy9libf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1lu53se</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Suggestions for full length tips</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lu53se/suggestions_for_full_length_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1lu4vgm</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Another nude almond set</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu4vgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1lu4q7k</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Engament nails!</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu4q7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1lu3nc0</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Whoopsies</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu3nc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1lu4hih</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>The weather has been super rainy and dreary here, so I needed something to make me happy</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oh87696xdibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1lu4a2a</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Ombré love</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4oolvqkcibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1lu3q4a</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Before and after</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu3q4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1lu3h3o</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Did some Yoshi Nails for my trip to Super Nintendo World 💚</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ebfjnm07ibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1lu2rxc</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Please mourn with me</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu2rxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1lu2kvq</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>I think I almost ripped my nail off.</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jl8ax4kw0ibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1lu2gd1</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Umm what is happening?</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9funeqz10ibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1lu26se</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Praying to the nail gods</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu26se</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1lu2uzq</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Opinion on Beetle gelpolish?</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lu2uzq/opinion_on_beetle_gelpolish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1lu2olj</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Fanta/Orange Crush/Creamsicle</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu2olj</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1lu2o3r</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Minty Nails 💅💚</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgw7khqg1ibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1lu2d91</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sk6nnjhhzhbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1lu2c5m</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Summery Purple</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu2c5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1lu28ei</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Diy nail glue</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lu28ei/diy_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1lu1yey</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>woof !! 🖤🤍</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vk6urjowhbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1lu1had</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Hyponychium regrowth</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu1had</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1ltv01h</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Tips or even wording to use for this?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltv01h</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1ltt5ji</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Looking for a mostly white with a hint of pink nail color</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ltt5ji/looking_for_a_mostly_white_with_a_hint_of_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1ltszgv</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>do these nails look not cured enough?</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltszgv</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1ltsbuk</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Acrylics uncomfortable while pregnant</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ltsbuk/acrylics_uncomfortable_while_pregnant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1ltqgaa</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>How to keep nails healthy while working in a kitchen?</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ltqgaa/how_to_keep_nails_healthy_while_working_in_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1ltwpoq</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Why is my gel nails peeling of?</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9f6g8qjdxgbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1ltzcv4</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>May I humbly suggest the rubber band twirl method for glass bead style magnetizing.</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/urvp4exbfhbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1lu1eat</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Been practicing how to do my nails</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fptj8ljoshbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1lu1e4a</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>First set of nails for my birthday month! 🎂</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lt1ma0gsshbf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1lu0rfp</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Strawberry shortcake set I did yesterday!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxf352poohbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1lu0lzf</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Trying out a flowy 3D effect</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu0lzf</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1lu0jse</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>She sells sea shells 🐚 🌊</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6eluon2anhbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1lu00pt</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>any way to fix this</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu00pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1ltzm6a</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>New set 🫧🤍</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khnt6753hhbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1ltyo72</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Sturdy as hell fake nails help!</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlwvaefrahbf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1ltxrws</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Fruit salad 🍓🥝🍋</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4poh12ar4hbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1ltx259</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Trying out floral nails 🌷</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nbme79jszgbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1ltwyks</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>My inch long nails broke and I had to cut them all 😭 this terracotta is quite cute on my shorties though</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kh8ywe3zgbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1ltwm74</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Naturals ki🎀</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z02of3eowgbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1ltwk9i</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Clear gel on natural nails</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ltwk9i/clear_gel_on_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1ltwdwn</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>How to prevent my nails from breaking?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltwdwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1luil4a</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>A England check-out issue</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77s3y12ztlbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1lui37l</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>... For Science!</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y7oi3rnwnlbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1lui2dl</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>ok emily de molly fans. you've got a convert</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lui2dl</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1luhh2a</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Great customer service</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6w13rp8mglbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1luhd7w</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>My first indie polish!</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1luhd7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1luhcyg</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>My first indie polish!</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s13cpupbflbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1luhb74</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>flowers in a pond but it’s stars in a rainbow</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4dtetyrelbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1lugygy</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>And they call her Sandy Claaaaws</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lugygy</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1lug8cz</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Help me ID a childhood nail kit?</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lug8cz/help_me_id_a_childhood_nail_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1luf6bt</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Nail strengthener/base suggestions</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1luf6bt/nail_strengthenerbase_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1luf59b</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Maybe We'll Learn to Be Kind - stunning!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vimjkg22rkbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1ludnhj</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Did I dupe myself?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ludnhj/did_i_dupe_myself/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1lud77p</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Petals for a Narcissist on my freshly cut claws</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lud77p</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1lucvc4</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Forces n F ields</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lucvc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1lucrg8</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>KB Shimmer - Pitcher This 🩷</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lucrg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1lucojc</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Can never go wrong with blue</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxn4sjbe5kbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1lucfi1</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Ode to BKL Lemon</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2er51da63kbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1lucejy</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Guess the movie 🍿</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3s0wy1ly2kbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1luc73l</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>In shock 😍</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1luc73l</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1luc3qy</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Neutral dip powder combos have me in a chokehold 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g3cphqj90kbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1lubial</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>What the heck is this peeling/scaling?</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19163nv6vjbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1lubhpn</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>With A Broken Heart-Pahlish (hospital lighting from a non-patient included)</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lubhpn</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1lubek9</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Does anyone know the name of this type of style/ how it’s achieved?</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lubek9</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1lub7r8</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Mooncat top coat stringy?</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jg68h2vosjbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1lub76g</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>My Bees Knees mystery prototypes</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lub76g</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1lub41r</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>b•color Watercolor effect top coat. Anyone else tried these?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lub41r/bcolor_watercolor_effect_top_coat_anyone_else/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1luaw3n</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>My first thermal! Paradox Polish - I Will Survive (PPU June ‘25)</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfnrxkuypjbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1luar8l</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>pastel teal/minty green with a hot pink shimmer - any reccos?</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7pdgbhsuojbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1lu9znj</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Wanted to share my nail progress over the past year! 🍏</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu9znj</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1lu9vfr</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Scared.  Dermatitis symptoms from regular polish? (Tagged nsfw to be but it's just a few bumps, not gory)</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu9vfr</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1lu9t1r</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Trying to dupe Labradorite from the By Dany Vianna/Vanessa Molina/whatcha Zodiac collab</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu9t1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1lu9jo9</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>The many faces of FTS</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu9jo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1lu8stt</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Summer Greeeeen!!</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu8stt</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1lu85hz</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>When a haul comes in, do you wait to put them on or immediately take off your current mani?</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pishhh8z3jbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1lu7pi7</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Mooncat Moonflower vs ILNP Mega (s)</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b2b9mppk0jbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1lu7mcj</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Someone had asked for this combo</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu7mcj</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1lu7lgg</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>The polish shades I pick vs the shades my husband picks for me</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xxdczutzibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1lu7bph</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>a magnetic charcuterie board</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu7bph</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1lu746p</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Professional yet pretty Pink Suede</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d9whm8l8wibf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1lu6x67</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Your favorite light/medium more purpleish blurples</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lu6x67/your_favorite_lightmedium_more_purpleish_blurples/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1lu6pua</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>representing those of us who still only have bar magnets lol</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9n3q3sictibf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1lu6cxe</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Lust for Vengeance</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu6cxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1lu63nt</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>I’m so in love with How Noble by Kbshimmer !!!! The blue &amp; green flakes make me think of earth 🌎🌍🌏 :) hard to capture all of its beauty in pics</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu63nt</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1lu5655</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>More circling magnet delights</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zvcq2gumiibf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1lu4ilh</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Poly nail gel?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lu4ilh/poly_nail_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1lu4iip</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>So happy with Lynb's Enigmatic Glow!</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czatsi9sdibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1lu4cjo</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Midsummer Eve is so pretty velvetized ✨️</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rr72dv30dibf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1lu43sj</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>I Scream Nails- Do You Party</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu43sj</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1lu3n5m</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Random combination I ended up liking quite a bit~</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncr2npgs7ibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1lu2qwo</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Found my Holy Grail QDTC...</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lu2qwo/found_my_holy_grail_qdtc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1lu2lir</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Advice for improving nail health</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu2lir</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1lu2kfg</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Never forget how pretty Live Love Polish is… was? Whatever. Look at them.</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzou3jwt0ibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1lu20n6</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Light purple with blue/green shimmer comparisons</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu20n6</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1lu1u39</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>touching up a mani - QDTC or regular topcoat?</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lu1u39/touching_up_a_mani_qdtc_or_regular_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1lu1sii</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>When I use top coat (and fully wait for it to dry), it seems like my nail polish comes off faster. I tend to do two thin coats of polish beneath the top coat. Is it something with my approach, or is the sally hansen one not working for me?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lu1sii/when_i_use_top_coat_and_fully_wait_for_it_to_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1lu1rj8</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Why do some brands get “forgiven” more than others?</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lu1rj8/why_do_some_brands_get_forgiven_more_than_others/</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1lu1czc</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Acrylic, Gel, or Dip for Home Manicure</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lu1czc/acrylic_gel_or_dip_for_home_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1lu10zp</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>sunset color polishes recs</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lu10zp/sunset_color_polishes_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1lu0y8k</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>✨Fancy Fingers✨ HERMES</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ohp9siwphbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1lu0p2p</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>ILNP Twirl dupe?</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lu0p2p/ilnp_twirl_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1lu0ki6</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Fanta</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p7agy399nhbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1lu04s3</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>KB Shimmer base coat opinons</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lu04s3/kb_shimmer_base_coat_opinons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1lu03x1</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Eddie gel or speed setter?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lu03x1/eddie_gel_or_speed_setter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1ltz89e</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Fireside🔥</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltz89e</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1ltz6vb</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Obsidian Orchid 💜🩷</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wsuzo889ehbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1ltz6sw</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Queen of the dead 🪾 👑</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltyvw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1ltz5y2</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>May I humbly suggest the rubber band twirl method for  glass bead style magnetizing.</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/clpj4802ehbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1ltyzwx</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Office lights are not your friend</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltyzwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1ltywz0</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>All I want to wear and say these days 🫠</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5q1828dechbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1ltytdq</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Need help figuring out what product was used and how to  remove it.</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ltytdq/need_help_figuring_out_what_product_was_used_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1ltyguh</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Nail mail arrivals lead to some interesting manicures !!</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4nyzrasf9hbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1ltxmwk</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>swatch sticks?</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ltxmwk/swatch_sticks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1ltx972</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Light and bright</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltx972</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1ltwk5j</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>DO NOT ATTEMPT!!</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5oheyrr1wgbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1ltwewl</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>I normally steer clear of anything resembling grey as they wash me out, but ILNP Pitter Patter is super complimentary</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltwewl</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1ltvsvz</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>My first PPU disappointment ☹️</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltvsvz</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1ltvhz9</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Good vs Wicked</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9ffuzpvogbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1ltv53d</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>I ruined my nails in 2 years and now  I am heartbroken.</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ltv53d/i_ruined_my_nails_in_2_years_and_now_i_am/</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1ltv1ks</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Two times the fun</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltv1ks</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1lttmbt</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Barry M shade ID please?</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lttmbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1ltsr7a</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Dupes for LynBdesign - I crave Star Damage?</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltsr7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1ltseee</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Sad Wedding Day Help &amp; Advice Needed pls ☹️</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ltseee/sad_wedding_day_help_advice_needed_pls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1ltsbbz</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Loving how this combo turned out</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yrp119iezfbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1ltkea5</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Help identifying this OPI shade</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltkea5</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1lti228</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Dupe request for lights lacquer</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lti228</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1ltmgok</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Mermaid bait vs hilt</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltmgok</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1ltq8qs</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ltq8qs/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1luhuic</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Click-on nails</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1luhuic</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1luhd57</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Did these myself to match a dress I bought</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1luhd57</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1luh3hr</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Hand-painted</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3cvozbx4clbf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1lucpgp</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Flower cateye 💅</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7jhqv1m5kbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1luf4im</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>I love making these types of designs</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rghj4hmhrkbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1luel29</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>these vacation nails i just finished 🥹🖤</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1luel29</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1ludlft</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Today's thing ✨️💅</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcmb9e3edkbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1lubn75</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Summerween nails for a friend of mine</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uhtupa29wjbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1luabej</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>First nails and my most recent one, edit/und-edit(beginner and doing homemade press on/I don't mind advice)</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1luabej</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1lu9pqs</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>vacation nails!!</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0umntnp7gjbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1lu8p59</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Practice on cheap fake nails</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b07r4va58jbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1lu7jyh</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Cat eye cherry blossoms 🥰🌸</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qop1v5izibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1lu7bmj</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Playing in My Sister nail polish’s</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu7bmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1lu6rux</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>freehand lettering press ons 🎱</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p51kf0qttibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1ltwzd5</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>first time posting, definitely nervous 🥺</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltwzd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1lu44t6</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Magnetic effect on a champagne color</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u992acskbibf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1lu2jmr</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>First Time w/ New Tech</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lu2jmr</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1lu1vxt</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Best way to take off foil from gel liner pots?</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lu1vxt/best_way_to_take_off_foil_from_gel_liner_pots/</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1ltzq7k</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>My work, what do you think??</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltzq7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1ltveco</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Confetti nails</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ltveco</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1ltrsvk</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Simple but beautiful design, artist @renovarte_studio</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/en3kdf0fufbf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1ltp70z</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>that DAWG in me</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74dz0pl52fbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jul 10 08:13:13 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_13.xlsx
+++ b/data/collected_data/2025_07_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C710"/>
+  <dimension ref="A1:C923"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12503,6 +12503,3627 @@
         </is>
       </c>
     </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1lw6zjv</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>red for envy. is it said? ♥️😂</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9obe0ou760cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1lw69ik</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Summer nails 🫧🌸</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lw69ik</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1lw66ql</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Jurassic Park nails! 🦖🦕</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lw66ql</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1lw5zu8</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Is it okay to go in for a fresh set?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjuh4xwauzbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1lw4zdz</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Should I throw out the products I used?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lw4zdz/should_i_throw_out_the_products_i_used/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1lw5g1a</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Help with good acetone brand for removing gel!</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lw5g1a/help_with_good_acetone_brand_for_removing_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1lw4ynb</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>how to make press ons actually last?</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lw4ynb/how_to_make_press_ons_actually_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1lw45vj</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Neon Green nail polish</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lw45vj/neon_green_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1lw2xxt</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Looking for nail service advice</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lw2xxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1lw4jk0</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Before and after 💅🏼</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lw4jk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1lw3zhc</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Asking for price quotation</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lw3zhc/asking_for_price_quotation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1lw34vl</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Got chrome nails for the first time, are they supposed to be see-through?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lw34vl/got_chrome_nails_for_the_first_time_are_they/</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1lw3376</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Time to say goodbye 🥲</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lw3376</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1lw2o03</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>What I asked for, what I got</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lw2o03</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1lw2twz</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Cat’s eye</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsyv67cvwybf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1lw1t30</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Attempted a white French, it’s not perfect but it’ll do</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lw1t30</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1lw1mep</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>First time trying press ons - are they crooked?</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lw1mep</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1lw0bte</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lw0bte</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1lvzn1z</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>First time press-ons</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvzn1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1lvz3mj</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>what happens to ur nails after a repair?</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lvz3mj/what_happens_to_ur_nails_after_a_repair/</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1lvzhnz</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Summer neons ☀️💗🧡</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yw0jdz0y2ybf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1lvzetp</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Italian horn manicure</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvzetp</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1lvzcyj</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Something playful for the summer ✨</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4au8r3ws1ybf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1lvz8n8</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Did my nail tech do a good job?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvz8n8</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1lvyomg</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>kiwi dragonfruit nails!</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69xqr17yvxbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1lvy6v4</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Online Nail Tech School</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lvy6v4/online_nail_tech_school/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1lvxrr4</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Recommendations for wedding nails for an absolute beginner / ex nail biter?</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9u5rkbgoxbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1lvxl6e</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Couples Toad &amp; Toadette nails ❤️🤍🩷</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvxl6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1lvxbnz</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>My tech wanted to branch out on her style so I let my nails be the tester 🌀🌀</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c7rntllukxbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1lvxac7</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Tips on how to prevent side splits?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kot31uakkxbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1lvx6lh</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>I love pink 🩷</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gg0ura1qjxbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1lvx1b1</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Asked the salon if they can do this in 40 minutes and two nail techs made it happen !!!</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fba8c7tjixbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1lvwr5p</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Mooncat - Moonflower</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvwr5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1lvwacs</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Should my nails look like this after soft gel removal? And how do I improve for my right hand?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvwacs</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1lvuf68</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>My tech just constantly delivers stunning work</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvuf68</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1lvttl2</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Help with opal nails?</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3j1zsqruwbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1lvtjso</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>I've been working on my nail art. Please critique.</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvtjso</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1lvtafv</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Bad at nails</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvtafv</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1lvt7xf</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Indents in nails</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvt7xf</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1lvtkkd</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>a set my newbie sister did! she’s getting so good.</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d5716s50twbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1lvtfy9</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Did she do me dirty?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqpv3bw2swbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1lvsk4n</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Russian mani</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvsk4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1lvrrru</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>What nails are those? (harlspoison on Pinterest)</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8unlcw3agwbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1lvs6j9</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Poptarts ahh nails 😭🥲🩷</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvs6j9</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1lvs0mz</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Treated myself before my Mexico trip!</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onugkyf0iwbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1lvruf2</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>I asked for coffin &amp; although I love them, I’d say that’s square.. no?</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5l03edsgwbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1lvrt81</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Glue recs</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lvrt81/glue_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1lvrkjl</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Hello! Here's the cat-eye tutorial I promised. I hope you like it. 🥰</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/apojzovsewbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1lvqmi5</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Please rate my new work 🍄 what do you think?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvqmi5</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1lvqfq5</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Nails like Jewels 💎</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvqfq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1lvqep8</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Newest Nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z67rw4qp6wbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1lvq2u3</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Help required</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvq2u3</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1lvpsqj</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Dark nails on pale skin? Too harsh or the perfect contrast?</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cd1xef7k2wbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1lvplum</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Recent nails I’ve done!</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvplum</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1lvpjlt</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Does this nail shape suit me?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvpjlt</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1lvpbpl</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Best press ons and tips?</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lvpbpl/best_press_ons_and_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1lvp1wd</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>I love blue 💙</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3zerj3dxvbf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1lvokcc</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Summerween Frankenstein Nails</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmwaljk3uvbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1lvnouv</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>One of My favorites</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twm5bh13ovbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1lvnqjv</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Hello kitty &amp;  Kuromi !!!!!</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plcn4uueovbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1lvnp5b</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Builder gel at home!</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lvnp5b/builder_gel_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1lvmhsz</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Dip destroys my nails. Is it better to let it grow out than get it sanded off when giving nails a break?</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lvmhsz/dip_destroys_my_nails_is_it_better_to_let_it_grow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1lvnjmy</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>The sweetest combination 🎀🍒</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmm2qut2nvbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1lvh0b4</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Post-gel trauma</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lvh0b4/postgel_trauma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1lvmb5p</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Stella inspired nails ☀️☀️</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvmb5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1lvnen2</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>gel-x nails i’ve done on myself.. what do you think?</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvnen2</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1lvn8be</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Going to go back and ask to fix - tips?</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvn8be</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1lvn89c</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>redemption (?)</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvn89c</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1lvn5t1</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Is this normal? First time getting builder gel.</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axwxmihdkvbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1lvmvb3</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>London affordable BIAB?</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzg90ii7ivbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1lvmqhi</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>How much to charge for these?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvmqhi</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1lvmfp2</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Second time ever doing gel at home</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1ps0ni9fvbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1lvm60c</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>this muted purple is to die for 🖤 (Jackie brand, color 023)</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f12pwbledvbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1lvlz04</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>trying out different nail art, I love the polka dots &amp; stripes the most :’)</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvlz04</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1lvluze</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>My gel mani skills progress</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvluze</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1lvkehj</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>A bit vampy</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/868hy43x0vbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1lvjpwy</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Jello jello peel off base steps?</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lvjpwy/jello_jello_peel_off_base_steps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1lvllfh</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>My summer nails :)</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6kr487d9vbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1lvkz99</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Drillbits</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lvkz99/drillbits/</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1lvkgsl</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Milky x Blue 💙🤍</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvkgsl</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1lvjxa4</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Looks different in natural light: yay or nay?</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvjxa4</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1lvjgwd</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>I'm working on this set, and need your help</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvjgwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1lvj90w</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Press-on</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvj90w</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1lvj7ng</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>So light and clean 🫧⚪️🤍</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cx9dw9vzrubf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1lvixfz</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Asked for something simple, thoughts on the length &amp; shape?</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bck515rrpubf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1lvintc</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>When do I know I need a fill in?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvintc</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1lvho9n</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Can black nails be elegant?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfabq7zifubf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1lvhnm5</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Showing off my fruit nails and my cat! 🍍🍓🍇</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nfg2g69cfubf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1lvhm4h</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Help :(</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uqkrbexpeubf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1lvguda</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/muiobh878ubf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1lvgqiq</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>🍋 summer vibes 🌊</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9ws4fv67ubf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1lvgm12</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Burgundy french cat eye with some gold</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvgm12</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1lvgk8r</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>OPI polish</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lvgk8r/opi_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1lvghd5</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Best glassy nail effect in Delhi!</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvghd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1lvg5qx</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Two parts: do I get my nails done? Do I get BIAB or shellac??</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5gtoqgj1ubf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1lver00</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Funky pink set 🩷</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jz5tx7jfmtbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1lveilv</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Beginner questions!</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lveilv/beginner_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1lve5o5</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>so obssesed w these tbh</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12lko0fgftbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1lvdqdn</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Non-lamp nails alternative</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lvdqdn/nonlamp_nails_alternative/</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1lvdplp</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Post exam celebration nails! Done by SnJ Nailroom in WA.</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvdplp</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1lw6qmq</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>mushroom nails 🍄😍</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsuuq90730cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1lw6oh0</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Ghoulish</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lw6oh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1lw553a</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>I declare this week to be immortalized as “Magnet Week” every year - who’s with me??</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lw553a/i_declare_this_week_to_be_immortalized_as_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1lw53i0</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>What nail color do you recommend?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zcsnsq4kzbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1lw41e7</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>How to create the glass bead effect without a horseshoe magnet, powered gadgets, or medical imaging equipment 🤓</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/xpPQcCH</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1lw3xxd</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Low tech glass bead attempt</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/er6ktr546ybf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1lw3fex</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Electric Nail File + Magnet = more spinny shenanigans!</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lw3fex</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1lw3dj3</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>More fun with magnets</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/llam8t632zbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1lw2pld</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Cuticle Remover</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lw2pld/cuticle_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1lw1b88</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Suggestions for jellie-like magnetics similar to MC Forbidden Fruit ?</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/piecz2zpiybf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1lw15zc</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Nail nerds at their finest</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kaj4g02dhybf1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1lw15m4</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Reddit La(c)querista Discord Polish!!</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lw15m4</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1lw11uc</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Hand mixer action shot- (on my thumb this time- was not flipping off!)</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l1nnszzegybf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1lw10p0</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Random Italian drug store polish</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lw10p0</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1lw0q38</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>So sparkly! So much rainbow!</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x5bgl1yjdybf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1lw0f23</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Pastel Holo Gradient</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozjkkp9waybf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1lw0cvi</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>The most interesting polish I own 🤩</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dbtj967caybf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1lw0c36</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Lilac Specialty Finishes Mani</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e7v4khh6aybf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1lw00fb</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Yet another spinny machine</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wwynurtc7ybf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1lvzzkb</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>June manicures</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvzzkb</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1lvzy7k</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>This thermal matches my keyboard 💕</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvzy7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1lvzu8i</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>ISO a black jelly with black flakies</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvzu8i/iso_a_black_jelly_with_black_flakies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1lvz6y7</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Endorphin mani</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybn2qved0ybf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1lvyyfq</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>MAC polish brush replacements</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvyyfq/mac_polish_brush_replacements/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1lvyizh</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Watermelon for the summer!</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvyizh</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1lvye19</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Pastel Yellow? in the golden hour sun</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rwxflx7itxbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1lvyapi</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Harvesting a Hard Drive Magnet (Plus Bonus Spindle)</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvyapi</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1lvxxha</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Giving yourself a Cock-a-Doodle-Doom mani makes crappy days less so.</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvxxha</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1lvxokh</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Can someone with access to an MRI machine please see what it does to magnetic polish</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvxokh/can_someone_with_access_to_an_mri_machine_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1lvxeq5</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Was thinking about hiring this guy to help with my mani's</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/px3hjg6jlxbf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1lvxamg</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>This wonderful sub</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b60pcupmkxbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1lvx0aq</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Jumping on the new magnetic trend bandwagon</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5itntpabixbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1lvx039</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Since we're going all in...</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/0d2kUO-2jd4?si=KtbJWVnuX0QBh3nI</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1lvwu0j</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>I bought these six crowstoes today for $1 each - just picked the colours I liked. There were a ton more. Should I have gotten the others?</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvwu0j</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1lvwthb</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Magnet safety</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvwthb/magnet_safety/</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1lvwbz7</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Taking bets (in make believe points)</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvwbz7/taking_bets_in_make_believe_points/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1lvw09s</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Clear/black thermal</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvw09s/clearblack_thermal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1lvvkk2</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>I think 8 hurt my husband's feelings 💅</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvvkk2/i_think_8_hurt_my_husbands_feelings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1lvvdfo</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>OK my turn!</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvvdfo/ok_my_turn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1lvv5nk</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Room for a thousand (cursed hand poses)</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvv5nk</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1lvukrg</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>My contraption. Low speed worked great.</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6kgptqw30xbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1lvucn0</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>As a newbie I've no idea what the magnets do, and at this point I'm too afraid to ask</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvucn0/as_a_newbie_ive_no_idea_what_the_magnets_do_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1lvsxgt</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>ILNP Gummy Bear + Glowstick creates glowy, summer vibes 😍💖🪼🪩</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u6l2kj3eowbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1lvswcg</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>ILNP Lily</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2h2e6xi8owbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1lvstf6</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>My first non creme yellow</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvsq9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1lvs4f6</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Giant Glitter Bombs circa 2011 - 2013</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvs4f6/giant_glitter_bombs_circa_2011_2013/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1lvs0u1</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>I've fallen in love with shifty polishes - plz send reccommendations</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/osye0g50iwbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1lvrvw6</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>glad i decided to move a little out of my comfort zone!</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/symanvm2hwbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1lvr8gm</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>First time doing velvet</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p6tk6udhcwbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1lvr0zb</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Not sure how I’m feeling about ILNP’s Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvr0zb</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1lvn6a6</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Similar to OPI Dance Party Teal Down?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvn6a6</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1lvqljh</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Feeling a Little Dizzy</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7prt0sby7wbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1lvpu6o</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>A View To A Thrill 🩷</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvpu6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1lvpou0</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>1,200lb magnet (DO NOT DO THIS. SAFETY FIRST)</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0y5jyzyr1wbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1lvpblk</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>My Bog Dweller arrived! 🎉</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvpblk</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1lvorwg</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>How to solve problem of dipping brush causing bubbles?</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6h7h4u85vvbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1lvon84</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Regular nail polish future</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvon84/regular_nail_polish_future/</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1lvo9db</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Cupcake Polish Skittle Mani</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwfe1171svbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1lvo8a9</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>My horseshoe magnet lost it’s power but here look what happens with bar magnets</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lqlnuryqrvbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1lvo1br</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Okay L.A. Colors - Calm Down! 🌠</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/53snk3eipvbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1lvnuui</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>My favourite Flower Child Combination so far!</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvnuui</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1lvnb54</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>With all these magnetic contraptions...</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvnb54/with_all_these_magnetic_contraptions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1lvn0oo</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Cuticle guards that actually work?</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvn0oo/cuticle_guards_that_actually_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1lvmrvm</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Update: 95lb magnet… FOR SCIENCE</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ereu1frkhvbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1lvm7lk</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Texas Flood Relief Charity Polishes</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wkpoldpdvbf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1lvlw32</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Lumen Hidden Bookshop</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvlw32</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1lvlu8k</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Nails of the day</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6yhol192bvbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1lvltnw</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>🏝️Beach Nails</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvltnw</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1lvlp1a</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Do I need sour apple rings?</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvlp1a/do_i_need_sour_apple_rings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1lvli6t</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>How it started vs how it’s going 💅🏻</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvli6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1lvkbdt</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Is this… too much?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8i13kta0vbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1lvkbb7</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Mooncat - Garden of Evil</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/34bivi7a0vbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1lvh17a</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>My graduation nails</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m33wkxuw9ubf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1lvjupy</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Sunset Lazy Gradient</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/27t36vnpwubf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1lvj779</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Dupe for these types of polish?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvj779</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1lvilb7</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Is there a PPU Reddit Community?</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvilb7/is_there_a_ppu_reddit_community/</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1lvicve</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Mooncat root of all evil ft. school floor</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llsrg159lubf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1lvi5hq</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Lurid Lacquers Schneewittchen really is THAT GIRL</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zu10m2d4jubf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1lvi3ph</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>This satisfied my orange craving nicely 🍊</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvi3ph</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1lvhhzo</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Some Dupe requests (PPU/HHC)</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvhhzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1lvcee8</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>First time getting my nails done [26M] - What's the verdict? 😅</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i5s7pr21usbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1lvgo94</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Magnet + Milk Frother</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/68eyo1bg6ubf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1lvghdh</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>I felt like I waited FOREVER to get my hands on this and I'm so happy it's finally mine.</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uvnk0lsn4ubf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1lvgcgl</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>I found my wedding nail polish! Cirque Colors Lavender Sky</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvgcgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1lvg1m8</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>I swatched my collection and here is my top 5!</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvg1m8</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1lv31qv</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>How do I stop biting my nails???</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lv31qv/how_do_i_stop_biting_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1lv9t78</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Spinning Disco Ball Motor</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lv9t78/spinning_disco_ball_motor/</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1lvfdv3</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>New sub anthem</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/re1upnicttbf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1lvfdfh</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Summertimeeee</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvfdfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1lvdy9h</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Dupes</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lvdy9h/dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1lvrenp</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>3D squiggle/swirl set!</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yv2mmwhqdwbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1lw32a0</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Hawaii vibe 🌊☀️</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9b7jd434zybf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1lw3173</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Work at home</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4nhvottyybf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1lvzpi2</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Can an actual nail artist please let me know what I should have asked for?</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvzpi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1lvz56o</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Summertime nails</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvz56o</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1lvxzml</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Uñitas que hice hoy 💅</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvxzml</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1lvx8ty</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>summer vibes💛🩷</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvx8ty</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1lvw4vp</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>This year’s birthday nails!!!! This isn’t just a new set, this is art🤩 Who can spot in them how old I am today?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mv8kkl3kbxbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1lvw2xe</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Tried acrylics for summer at Le Belle Nails &amp; Spa – here’s my honest take 💅</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4b7yx95bxbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1lvw103</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Isolated chrome stamping</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzrf1w2raxbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1lvt1y5</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Fairycore Mushroom nails! 🍄🌿</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvt1y5</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1lvsubr</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Help needed</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvsubr</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1lvsc4b</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>lava lamp nails i did!!🌈</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ryt59adakwbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1lvs64t</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Today's work</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzzgdoe4jwbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1lvqqn5</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>pearls for nails that aren’t half back?</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lvqqn5/pearls_for_nails_that_arent_half_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1lvnzgq</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Nail art starter kit?</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvnzgq</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1lvm7gi</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>How do you keep matte white clean?</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lvm7gi/how_do_you_keep_matte_white_clean/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1lvm19i</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>practicing nail art, I love the polka dots &amp; stripe patterns❤️❤️</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvm19i</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1lvli8b</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Just a quick set</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7t4576r8vbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1lvkahd</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>klimtnails 我好喜歡🥰</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o4hkr40wzubf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1lvjfsb</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Made these recently, def not perfect but I’m pretty proud of myself 💕</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lvjfsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1lvh04w</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>My work 🦋</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7qh993n9ubf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1lvfvv4</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Why is my chrome getting stuck around my art?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9wapf7opytbf1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jul 11 08:13:08 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_13.xlsx
+++ b/data/collected_data/2025_07_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C923"/>
+  <dimension ref="A1:C1138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16124,6 +16124,3661 @@
         </is>
       </c>
     </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1lx14wu</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Wanted to share how cute my nails ended up and thought this was the place</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6tbub40c7cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1lx0dqe</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Progress pics! Im really proud of myself</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx0dqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1lx0cx7</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Cajun shrimp dupes??</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lx0cx7/cajun_shrimp_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1lx0bxr</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Wtf is that</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx0bxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1lwzf9k</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Next set</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjen2gh7s6cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1lwy1jd</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>First time using builder gel!</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwy1jd</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1lwxjxh</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>How to achieve these beautiful glossy aqua nails? (the picture is TOGZOM press ons)</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dt2rln1r86cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1lwygo4</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>New nails 🐞</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfg08amuh6cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1lwyaai</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Sunflowers and roses</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwyaai</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1lwxw76</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>I saw them and fell in love, next set 😍❤️</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sy6h8a2c6cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1lwxvvw</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Give me your DIY french nails tips!</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwxvvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1lwxsc7</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Beach nails</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inz4g2i0b6cf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1lwxgfi</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>My nail tech slayed</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9t80omkt76cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1lwxbcj</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Fresh mani ✨️ 💅</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjcjdsfg66cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1lwx9mo</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Fresh set</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7mstpyz56cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1lwwd4y</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>How to remove nail extensions residue? Tried at home</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2siiprokx5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1lwwb17</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Which one is your favorite?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwwb17</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1lwwa4p</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>How did i do?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwwa4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1lww24i</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>First ever acrylics, is this redness at the base of the nail normal?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lww24i</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1lwvvwm</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Watermelon nails ❤️ 🍉</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdcem8w6t5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1lwvg59</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Good low-cost e-file for personal use?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lwvg59/good_lowcost_efile_for_personal_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1lwvcem</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>My new set (pressons)</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0w64p4mio5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1lwv92x</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Glitterbels Questions</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lwv92x/glitterbels_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1lwuvrg</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>should i be worried?</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwuvrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1lwv5lz</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Holo taco moon lagoon and garden party taco</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pax0v4hvm5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1lwuu52</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>My new nail tech went HAM on my cuticles, is this normal these days?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lwuu52/my_new_nail_tech_went_ham_on_my_cuticles_is_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1lwv3f9</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Apres wtf</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwv3f9</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1lwuzxu</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>What do you think of these?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwuzxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1lwux75</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Long Square Set in a Semi-Transparent Red Tint 💅</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwux75</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1lwtn8a</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Gel and rhinestone manicure inspired by Lady Gaga's The Fame</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/708ot2cq95cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1lwupwe</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Pink nails, coffee, and mountains — the perfect combo</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mk47w6l3j5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1lwuor5</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Help with see-through French nails</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnmyu8rji5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1lwulwi</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>What should I do?!</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lwulwi/what_should_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1lwuijf</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>My summer nails</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ctxyulqah5cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1lwud1n</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxd0w5g0g5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1lwua0f</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Out of this world</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwua0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1lwtz6m</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>I 💛 my nail tech</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ugb1ojnc5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1lwts95</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>First time nail art (Pt 2)</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwckhs9ya5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1lwtnk8</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Aurora Aura ✨</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwtnk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1lwtfns</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>made my nails shorter and hate them help</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwtfns</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1lwssuo</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Expectation vs Reality</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7beb8s115cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1lwsfud</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Colorful</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8mbre4zy4cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1lwsxvt</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>New Color and Gel!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwsxvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1lwt2bt</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>I ✨FINALLY✨ had a positive experience getting my nails done!</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwt2bt</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1lwtass</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Favorite press ons ever 🤎</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ja5h0ip65cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1lwta79</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>My “professional” gel manicure rant - why oh why 🤦🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lwta79/my_professional_gel_manicure_rant_why_oh_why/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1lwt90s</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Got chrome nails for the first time — are they supposed to be see-through? Inspo from @marynethibarrie on pinterest</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lwt90s/got_chrome_nails_for_the_first_time_are_they/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1lwt06d</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Gold flake opal moment</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwt06d</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1lwsxve</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Lifting acrylics</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lwsxve/lifting_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1lwn28m</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Bee themed Press On’s- which one would you buy/wear?</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hj3n41f2v3cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1lwn10w</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>For those who developed acrylics allergi, how do you do your nails now ? what products do you use ?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lwn10w/for_those_who_developed_acrylics_allergi_how_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1lwm9mx</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Camo nails 💕</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vrszb5cjp3cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1lwqt9l</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Acrylic nails lifting on vacation (help pls!)</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lwqt9l/acrylic_nails_lifting_on_vacation_help_pls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1lwrdat</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>I can’t figure out why these look bad</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k57mnw1pq4cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1lws5xo</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>I got Cherries 🍒 🍒</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lws5xo</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1lws5ox</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>My natural nails before &amp; after</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lws5ox</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1lwrzk3</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>My nail art book</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2z7dsgmv4cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1lwroyk</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Sunset aura🍊✨💖🌅</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwroyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1lwrfvd</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Are these even or am I just paranoid</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nr04b7w8r4cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1lwrb4l</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Is it supposed to look like this?</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5zfx3e17q4cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1lwqqwh</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>elegant white</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4a950d6yl4cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1lwqjm7</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Did my own nails for the first time ever</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwqjm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1lwq3o6</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Why didn't I try this sooner?</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwq3o6</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1lwq2ys</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>My husband picked the color</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujspfh0wg4cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1lwq0c8</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>So fun! 💅</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5mdhk0mdg4cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1lwpmoa</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>❤️‍🔥❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wibnf44kd4cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1lwphs4</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Can I still go to my appt??</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwphs4</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1lwpapw</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>I wasn’t happy with my last ones so I knocked these up quickly and I muuuuuch prefer them!</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zepy4n2b4cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1lwoxg6</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>French ombré w chrome top and hibiscus flower builder gel</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwoxg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1lwo11l</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>🌺 🌸</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwo11l</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1lwnzld</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>What shape is best for natural nails?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7m9hfmgj14cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1lwnmt9</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>What do you think about these?</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2dtdne0z3cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1lwnbai</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>My mom did my nails</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwnbai</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1lwnb1s</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Sheer/Translucent Polish</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lwnb1s/sheertranslucent_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1lwn6gf</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>My all time favorite set!</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwn6gf</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1lwmsxa</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>first and second attempts at painting my own nails 💅 😁 was better about the base and top coat in pic #2 and I'm happy to say they've stayed on all week. Got my first chip today though 🥲</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwmsxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1lwml2t</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Fair tip</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lwml2t/fair_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1lwmg7z</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Red stiletto stabbies</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwmg7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1lwlvnh</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Went shorter... did I fumble?</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwlvnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1lwlwpg</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Fresh set ✨</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjz93svxm3cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1lwlpt3</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>First time nail art (straight male)</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwlpt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1lwlo76</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Nails advice?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwlo76</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1lwlm6d</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>when to get biab nails redone?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lwlm6d/when_to_get_biab_nails_redone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1lwlc7r</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Are my nails just doomed?</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lwlc7r/are_my_nails_just_doomed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1lwcnsp</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Working at a pawn shop off dangerous…</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwcnsp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1lwl7sl</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Dollar Tree “Gel X” Nails with RCM</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwl7sl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1lwldmp</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Cute Froggy Nails</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwldmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1lwla5x</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>How they look now/how they looked two months ago</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwla5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1lwl70d</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>obsessed w my new set!</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1pry6qgth3cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1lwl6jn</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Got my first ever extensions today!</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwl6jn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1lwl4x8</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>3 months of growth</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwl4x8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1lwl2nb</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Does anyone have any tips for full coverage loose glitter nails??</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yg7gi2xug3cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1lwkvz7</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Tried something new and I love them!</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69jfb88if3cf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1lwksh9</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Nail design for my first nail commission!&lt;3</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwksh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1lwkc9p</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Summertime nails</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93jcusxvb3cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1lwk8i2</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Gifts?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lwk8i2/gifts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1lwj5pw</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Design Help - Vegas Inspo</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwj5pw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1lwiauo</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Struggling With DND Gel Removal &amp; Nail Damage — Need Help With My Routine</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lwiauo/struggling_with_dnd_gel_removal_nail_damage_need/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1lwk5te</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwk5te</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1lwjs1b</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Nailie Cutie Club</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzb4q16z73cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1lx14z5</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>🔮Wild Berry Fairy Skittle 🌸</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckwwtyz0c7cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1lx0owx</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Sorry I’m late, I was working on a solution for the gel mani crew</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ds5o46tj67cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1lx0cce</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Cajun shrimp dupes??</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lx0cce/cajun_shrimp_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1lwyo33</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Magnetic polish dispersion with KB shimmer clearly on top</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxrzlxqzj6cf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1lwynw5</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>This one’s my speed (spinny magnet post)</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l27mbrw4j6cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1lwyb56</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>First layering experiment I’m really happy with</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k0nol4nag6cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1lww4z8</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Thought I didn't like bright palettes, but neons + chrome = dopamine</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lww4z8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1lwvpop</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>The polish that makes you the happiest</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lwvpop/the_polish_that_makes_you_the_happiest/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1lwvn1t</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>You all are magnetic :)</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gqv3xd3r5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1lwur0m</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>My DIY Neon Collection</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwur0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1lwun58</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>This might be the sparkliest polish I own</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zp5i61afi5cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1lwu9qy</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Rainbow tipped Serpent Queen</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwu9qy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1lwu88f</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>I call it the "combining my interests" pose</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwu88f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1lwu3ba</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>At this point just put a bar stool on the counter....</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/whiuc8mod5cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1lwtsit</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Dupes for this BKL prototype?</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t74l7ah0b5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1lwts27</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>What polish brands get your stamp of approval?</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mycgqcmwa5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1lwtqdi</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Anyone remember Pure Ice?</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwil6pwha5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1lwtdyn</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>I want to host a nail painting party!</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6mrmabh75cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1lwsyiz</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>🧲💅</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzwbx1rr35cf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1lws2du</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>One more for the pile!</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hj5339v5w4cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1lwrzax</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>My husband took apart a remote control car and built this contraption for me. He's loving all of the posts!</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t5stbggkv4cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1lwr7z6</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Orange recs</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lwr7z6/orange_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1lwr7lk</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Summer Barbie Nails 💖🐬</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwr7lk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1lwqtr0</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Tried the marble effect with this teal color and some gold flecks</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwqtr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1lwq6cv</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>glass bead achieved, sans contraption</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lwq6cv/glass_bead_achieved_sans_contraption/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1lwq1z6</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>This green 💚</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/syq671lpg4cf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1lwpgh0</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>BKL magnetics, you will always be famous</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lzjm1to8c4cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1lwp9gy</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Will mani mag work with new method</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scdnjhjta4cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1lwp891</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Can you make money from just designing nails?</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lwp891/can_you_make_money_from_just_designing_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1lwp3kp</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>baja blasty vacation manicure ⛱️🍹ft. LA Colors!</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwp3kp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1lwou6s</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Blursed Cat</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2d8dxsu5j1cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1lwot64</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Searching for the perfect gold</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lwot64/searching_for_the_perfect_gold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1lwonxw</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Is it red or pink? Love it anyway 😆</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwonxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1lwomul</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Nail hardener - is it a skill issue?</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lwomul/nail_hardener_is_it_a_skill_issue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1lwo6v0</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>My 10 year old son is the best</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iw05oiky24cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1lwnq1q</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>ILNP Amber, 30 lb horseshoe magnet, and a drill</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/57szb6wlz3cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1lwnamt</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Some Bunny Loves You 🐇</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwnamt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1lwn2ud</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>My DIY magnet spinner</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gr90qdi6v3cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1lwmbz8</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>BKL Magnetics are great!</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9vu9x10q3cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1lwm7og</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>I love this community so much</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6vuyy9i4p3cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1lwm71y</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Matte Topcoat As Glitter Grabber?</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lwm71y/matte_topcoat_as_glitter_grabber/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1lwm1dl</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Baja blast, anyone?</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nfi1i8vn3cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1lwlzwq</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Playing with magnets and my untrieds</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2mipi7rjn3cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1lwlh33</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Do you prefer pure jojoba oil or oil blends for oiling your nails?</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lwlh33/do_you_prefer_pure_jojoba_oil_or_oil_blends_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1lwl9w5</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Feeling so ethereal and magical ✨</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwl9w5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1lwkl6q</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Matching my nails to my outfit for an event this evening 💜</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwkl6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1lwkifh</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>July 🔴</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xeruf4f3d3cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1lwki2i</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>I cant stop! I wont stop! Spiralizer method</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uk2hrkqxc3cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1lwjnm3</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Not so trendy anymore but that doesn’t stop the sparkle 💖</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4qe7w6473cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1lwjkvy</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>To my fellow laqueristas concerned about shipping thermals in the summer</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbb1b5xk63cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1lwj4fh</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Finally found the perfect yellow🌞</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwj4fh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1lwixzx</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>I humbly request counsel</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwixzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1lwircn</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Neon Green with Blue Shimmer Comparison</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwircn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1lwigm7</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>DAM - Year of the Dragon</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwigm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1lwi90k</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>First time using a peely base. Any tips?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u249sp6ix2cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1lwi052</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Is it a bad idea to buy a Bisley or a Helmer?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lwi052/is_it_a_bad_idea_to_buy_a_bisley_or_a_helmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1lwhymx</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Favorite glitters?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lwhymx/favorite_glitters/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1lwhah8</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>My first Solar Polish! ☀️</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lomwfcmtq2cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1lwh7it</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Slice of Life</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sbrulpg8q2cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1lwh68f</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>What’s the actual difference between a velvetized magnetic polish, and a glass bead magnetic polish?</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lwh68f/whats_the_actual_difference_between_a_velvetized/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1lwh4gb</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>If they only knew the you that we know…</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwh4gb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1lwg6vm</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Dupe For Orly Blazing Sunset</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1u5si51j2cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1lwgljx</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Mooncat Gates of Hell</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwgljx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1lwg8pm</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Whispers of Camargue🌡️☀️</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwg8pm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1lwfubm</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Why did I sleep on this polish??</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5qndikmkg2cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1lwf995</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Attempt at duping Merkitten</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwf995</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1lwf261</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>reminds me of shiny seashells 🐚</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwf261</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1lwec7k</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Cuticle Care</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lwec7k/cuticle_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1lwd9ql</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Not me realising I'd done a glass bead technique without realising it a few months ago!</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/432uo4cx36je1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1lwd7a9</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>rip my long nails</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwd7a9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1lwcnxj</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>My first glass bead attempt and low-tech setup.</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x8h1avd5t1cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1lwc25p</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>One of us! One of us!</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s96cqqb9o1cf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1lwahm7</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>More lego magnets!</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uh0heqzu91cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1lwbnxd</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Split nail repair isn't holding</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lwbnxd/split_nail_repair_isnt_holding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1lwalig</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>This pink nail adhesive is insane! Stayed on for 3 days—even after washing hands. Have you tried it?</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tc9ko7s4b1cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1lwayju</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Hybrid Nails Question</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lwayju/hybrid_nails_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1lwazig</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>What am I missing in my collection?</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwazig</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1lwayd9</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Saw someone else post cherry nails here, it's my turn!</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwayd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1lwaett</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>EFile Magnet Spinner</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jse3kqh891cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1lw0jwz</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Any advice for a beginner who wants to make press ons? :)</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lw0jwz/any_advice_for_a_beginner_who_wants_to_make_press/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1lw3eea</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Does a U-shaped magnet need a magnet at the bottom or just the sides for velvet?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6x7fx962zbf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1lw8ugb</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>HHC Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lw8ugb/hhc_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1lw8qt7</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Always liked the look of nail art but I have such weird ugly nails that I never bothered. Anything I can do to improve them?</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lw8qt7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1lw8loy</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Couldn't help myself</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lw8loy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1lx16ov</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>How am I supposed to match this on my right hand 😅</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx16ov</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1lx0gei</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Hunter X Hunter full set, what your thought ?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx0gei</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1lwzn1h</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>one of my first nails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jt2wpucju6cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1lwgotv</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Beginner nail tech</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwgotv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1lwyn1r</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Flowers</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwyn1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1lwxacs</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Guess where I wanna be 🐠🦀🪸🪼</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwxacs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1lwvx97</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>first time my flowers turned out nice :)</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgo4rookt5cf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1lwv2xy</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>What do you think of these?</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwv2xy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1lwuufo</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>She wants all the colors 😂</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wttn01d6k5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1lwu902</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>One of my first custom sets!</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6x1nxm62f5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1lwu0z6</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Sculpted flower(?)</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sdvxtuk3d5cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1lwte4t</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Sculpting gel and pigment powder advice</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lwte4t/sculpting_gel_and_pigment_powder_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1lwsjob</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Nails with this vibe&gt;&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwsjob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1lwphex</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Some oranges for summer🧡🍊🏵️</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwphex</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1lwp98i</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Love doing lil ornamental designs on myself 🪲</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwp98i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1lwornq</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>If not Beetles what should I get!</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lwornq/if_not_beetles_what_should_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1lwmc42</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Bright colors have me in a chokehold during summer 😩</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6nj1e01q3cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1lwln3u</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>A friend got these nails done in this blue color and I loved them! Credits - martina.nails</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xoy4a2i0l3cf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1lwl1v2</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Nails for Tyler, The Creator Concert</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qi4gazivg3cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1lwkw6d</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Pastel acrylic nails :)</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwkw6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1lwjrgz</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>My first time using 3D sculpting gel!</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2wdt1jkv73cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1lwitty</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>How to reapply/reinforce fragile nail charms?</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egk5kfvg13cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1lwi8zn</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>First time getting acrylics as a straight guy!! What do the women think??</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwi8zn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1lwhqbk</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Nail tech work by Apple pink nails in va</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o54pnq1yt2cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1lwfr5j</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>How are you?</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ej704o5yf2cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1lweaxp</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Help with jelly look!</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lw823gdi52cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1lwdzk0</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>i'm still learning, but I'd like to know what you think or some advice. 🥰🥰🫶🏽🫶🏽🫶🏽</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwdzk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1lwaw2c</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>hello kitty ₍^. .^₎Ⳋ🎀</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lwaw2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1lwar3r</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>This pink nail adhesive is insane! Stayed on for 3 days—even after washing hands. Have you tried it?</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/buofi8lnc1cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1lwa5xy</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Blue Summer nail, I did it!💙</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hxt1vcv61cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1lw9xgj</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>New design</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05roth9f41cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jul 12 08:11:18 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_13.xlsx
+++ b/data/collected_data/2025_07_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1138"/>
+  <dimension ref="A1:C1337"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19779,6 +19779,3389 @@
         </is>
       </c>
     </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1lxv5gc</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>How to fix crooked nails</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxv5gc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1lxud57</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Is it possible to fix my nail?</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxud57</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1lxsuin</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Are natural nails still a thing?</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ls3kgtjsdcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1lxsof4</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>It was time for a change today</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxsof4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1lxroa3</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>My nail tech is honestly my best friend, she deserves an edible arrangement 💐</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyav3akdgdcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1lxro7n</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>First time getting French tips</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9vcupscgdcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1lxr5lr</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>2013 Sally Hansen -wavy blue</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxr5lr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1lxqspq</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>A gorgeous flower set I tried</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxqspq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1lxqga5</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>POV: you stopped biting your nails</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9x8rr0qe4dcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1lxq6c8</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Matte nail strengthener?</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lxq6c8/matte_nail_strengthener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1lxpm4b</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Blueberry lemon nails for summer</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9e21858cwccf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1lxoxfh</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Well, yes!</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ee6fhhivpccf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1lxpcev</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Hotdog theme nails! Handmade by me!</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxpcev</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1lxoxb6</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>My mother’s contribution for shark week</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5e71lqavpccf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1lxowkh</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>practical nail protection help</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lxowkh/practical_nail_protection_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1lxohqn</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>recently moved from an area where i wasn’t charged for gel soak offs to an area where they charge $20-30</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lxohqn/recently_moved_from_an_area_where_i_wasnt_charged/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1lxoe6j</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>I just keep staring at them</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxoe6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1lxob2u</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>ahh i’m in love</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxob2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1lxo857</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>particularly proud of when my natural nails got to these lengths!</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxo857</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1lxo6o6</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Etsy recs for glue press on's in solid colors?</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lxo6o6/etsy_recs_for_glue_press_ons_in_solid_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1lxlp47</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Broke my nails doing Brazilian jujitsu, gotta rock the short style now!</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxlp47</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1lxo2pn</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>I got my nails done for the first time today and something tells me it's not normal</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9wxnlkh9iccf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1lxnlfv</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Help &amp; Advice please</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lxnlfv/help_advice_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1lxmmqy</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>How to remove burn marks?</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ntmdw4kj5ccf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1lxmpxh</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Concerned</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrisdo9b6ccf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1lxo0jt</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Tired of short nails</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bof4sbdqhccf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1lxnm3n</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Bday Nails :33</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mfu33m54eccf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1lxnc28</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>finally found the perfect butter yellow!</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hdewlnqbccf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1lxm6kq</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Heart nails ❤️</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxm6kq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1lxm5s8</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>princess nails</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/npjvslhk1ccf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1lxm50w</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>SUN UV 2C lamp</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lxm50w/sun_uv_2c_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1lxloln</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Overdue Refresh💜</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxloln</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1lxl5d9</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>My new set</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxl5d9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1lxl0ci</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>all different greens 💚</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxub78sbsbcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1lxku09</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Why did this happen?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om3yq4rwqbcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1lxkoam</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Funeral nails</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjdpk3qmpbcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1lxkngb</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Fresh Nails and Jiu Jitsu Knuckles</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxkngb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1lxkn07</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>NAILZ 4 KE$HA</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jci0c5zcpbcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1lxkez7</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>White Pedi before hitting the beach 🤪⛱️ 🌞</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgzalzcjnbcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1lxk9hd</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Fun colors and texture</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxk9hd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1lxk4y1</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>New shape in lovely pink</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxk4y1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1lxk2s7</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Purple Cateye Starbursts</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plomz45ukbcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1lxjq1t</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Peachy keen 🍑</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyf87n04ibcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1lxjp3x</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>My girlfriend was told at her beauty college that this is a dehydrater, and so she uses it to dry out my cuticle for cuticle push backs and removal. Is that what this is?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxjp3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1lxj0js</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>do they look as good as i think?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x2weawtscbcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1lxiz06</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Best type of nail polish for damaged / thin nails?</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lxiz06/best_type_of_nail_polish_for_damaged_thin_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1lxitku</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>🧿</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mrqq9fdbbcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1lxirta</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Going to miss this set.</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hyte0pj0bbcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1lxh6d1</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Been seeing a lot of people posting about nail biting!</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxh6d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1lxhsul</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Recent set advice</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxhsul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1lxi5mg</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Pearlescent fuchsia (plus bonus golden hour pic)</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxi5mg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1lxi7cg</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Light Elegance Tack Bonding Agent</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lxi7cg/light_elegance_tack_bonding_agent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1lxi047</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Inky Chrome Freestyle 🩷 🖤</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zyrtyv185bcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1lxhyqf</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Vacation set 💅🏁</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ss9r5oe45bcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1lxhyj1</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Going to the bar to watch Love Island tonight.</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxhyj1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1lxhllo</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Barbie Pink nails 💅🏾 for vacation</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxo7iyfd2bcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1lxhebo</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>SOFT GEL TIPS + GLUE</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lxhebo/soft_gel_tips_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1lxh786</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>the most perfect manicure</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6k64u14jzacf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1lxh75b</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>My new claw work 🐾 What about this shape?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/db1kxunizacf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1lxgz12</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Polish and no polish :)</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxgz12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1lxgm7u</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Builder gel lifting</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lxgm7u/builder_gel_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1lxg8k6</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>I challenged myself to handpaint a Rumi nail set 😫 This art style has me in a chokehold</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bsg66uzksacf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1lxg7ni</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>my friend make a pretty long manicure for me</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2dh302fsacf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1lxg4h6</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Shaping tips?</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxg4h6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1lxg4ai</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>🌈 ✨ acrylic and gel</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxg4ai</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1lxfkaj</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>pomegranate &amp; lemon gel x 🍋💓</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxfkaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1lxfaig</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Not happy with my nails… am I overreacting?</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxfaig</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1lxftyl</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Perfect short French 💅🏽</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmvw4oiopacf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1lxfr77</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Which Shape?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxfr77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1lxfhst</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Are they doomed to always go up like this ?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxfhst</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1lxffw6</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Gel removal with jello jello</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lxffw6/gel_removal_with_jello_jello/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1lxezw7</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Lil dots</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxezw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1lxeuvn</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Mermaid Vibes</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxeuvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1lxeau3</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>How'd I do?</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxeau3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1lxe9ow</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Chrome is nice but I'm in LOVE with these sparkles!!</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1bahiroeacf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1lxe3mw</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Let it glow! 💅🏾</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxe3mw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1lxdwxi</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>New selfmade set for the summer🍒</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxdwxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1lxdrfh</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Press on nails for one night (fingers crossed they last)</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxdrfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1lxdqzz</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>natural nails with rubber 🌸</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pfvlfvb2bacf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1lxdde7</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>What I asked for vs what I got at the highest end salon in the city</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxdde7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1lxdcrs</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Can i seal my press ons like gel x?</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lxdcrs/can_i_seal_my_press_ons_like_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1lxd31q</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Which set is better for tortoise shell.. they both say tortoise shell…</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxd31q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1lxbumf</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Inspo + execution</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxbumf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1lxbfni</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Cotton Candy Clouds ☁️</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxbfni</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1lxbh46</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Old Fake Nails Art Ideas ?</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lxbh46/old_fake_nails_art_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1lx1ofd</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Is there any way to disguise regrowth under clear press-ons?</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0gvknaji7cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1lx68xs</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Is there a way to fix dried out nail polish that was accidentally left open?</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lx68xs/is_there_a_way_to_fix_dried_out_nail_polish_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1lx1vfq</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Cuticle help</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx1vfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1lx0kwo</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>nail biter to nail slayer 🗡️</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx0kwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1lxb75y</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Last Month’s Set 🌭</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pdt443pet9cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1lxb47v</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Not sure if it’s just nail polish or a whole galaxy holding on to me</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zk1ffpgus9cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1lxb0ai</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Dark red cat eye 🧛‍♀️ 🐈‍⬛ 🩸</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktjeuun2s9cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1lxaxwq</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Shape name?</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxaxwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1lxawcd</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Hangnail Care?</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5rfqrnbr9cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1lxahdg</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>In my ✨Chrome✨ Era</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxahdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1lxafgr</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>I feel like a princess</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxafgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1lx9q5s</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>How's it looking?!</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx9q5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1lx9dgs</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Acrylics</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx9dgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1lx8upe</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Practicing nail art on myself</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx8upe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1lx8sol</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Weekend nails</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/br7gioeqc9cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1lxu2ct</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Any non gel polish that looks like this?</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0bpte85s5ecf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1lxthmg</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Baja Blasted on white vs black base</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxthmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1lxst86</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Can we make a rule about magnetic nail post?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lxst86/can_we_make_a_rule_about_magnetic_nail_post/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1lxsjhp</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Broken nails, need help!</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pseemd4dpdcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1lxscpj</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Can it be done?</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xkvu4dendcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1lxrxa0</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Help me find this color!</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxrxa0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1lxqdkh</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>People of Color could use people’s help with stock.</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5573zyxn3dcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1lxqd16</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>What magnet can I use for non-gel magnetic polish?</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxqd16</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1lxpl41</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Hotdog Nails, for the Calgary Stampede! Made by me</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxpl41</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1lxpd6e</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Swatches - ring or book?</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lxpd6e/swatches_ring_or_book/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1lxovgj</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Chrome powder works on Olive and June super glossy top coat!!</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lxovgj/chrome_powder_works_on_olive_and_june_super/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1lxoqsg</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>New Favorite Combo Unlocked</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxoqsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1lxnsuf</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Indie Polish 10:02 Nails</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4mq6cfyqfccf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1lxnj5a</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>A pretty gnarly Etsy magnetic that I love/hate</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxnj5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1lxnaol</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>First fancy polish haul!</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxnaol</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1lxn99y</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Glowstick does indeed GLOW</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mk6jsg42bccf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1lxn15w</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Help. I did a dumb. How do I get this off?!</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxn15w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1lxmv4l</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Hopping on the magnet + lego trend</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxmv4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1lxkqo0</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Work is destroying my nails, help</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lxkqo0/work_is_destroying_my_nails_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1lxme7b</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>okay sassy sauce!! 🤩</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxme7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1lxm53l</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>I could no longer sit on the sidelines. In honor of magnet mania and in anticipation of shark 🦈 week I present my contraption</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxm53l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1lxl9pn</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Deep water skittle! I call it "A Sinking Feeling" 🌊</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02lhibe5rbcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1lxl029</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Dupe for the Cirque Colors current GWP?</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxoilhr9sbcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1lxkq64</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>A unique and special yellow</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxkq64</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1lxk6zk</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>And then there were the magnet fails…</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxk6zk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1lxk5yu</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>When it's ✨magical✨</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxk5yu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1lxk3vj</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Purple Cateye Starbursts</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g6jzeeu3lbcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1lxjtu4</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Going to see Superman tomorrow! 💙❤️</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxjtu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1lxjntx</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Polished for Days: UF-Glow and We Are All Just Stardust</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxjn7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1lxj7di</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Momo Yuyake is so beautiful</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxj7di</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1lxixqu</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>"Omg that's so pretty, is that gel?" Nope! 😁</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxixqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1lxim4n</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>I’m a bartender and lacquer isn’t doing for me and gel damaged my nails. 😭 Am I SOL?</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cimrebpu9bcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1lxij50</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>HELP! Old, unlabeled, and likely discontinued coppery color by OPI.</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxij50</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1lxi5nx</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Light Elegance Tack Bonding Agent</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lxi5nx/light_elegance_tack_bonding_agent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1lxi4p5</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Belated Mixed Feelings 4th of July Post</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxi4p5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1lxi180</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Air bubble?</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxgm3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1lxhjlg</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Saw these at Marshall’s and I’m still thinking about them</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uohcu7i12bcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1lxh89c</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Visible nail line!</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxh89c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1lxh2oq</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Joining the race with a Lego motor!</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9iijmfpjyacf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1lxgyda</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>I tried.</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zul8x39rxacf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1lxgtxe</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Tankfully Yours🪼💙</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ehn7kkkuwacf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1lxfwhk</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>My dual purpose magnet contraption</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0lp8wap6qacf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1lxfab4</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Doughnut shaped magnet?</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://a.co/d/1AaEcW2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1lxf50b</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Holoday on Apparition</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hr2nq2fukacf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1lxeohb</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>My Turn!</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dpq2skqhhacf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1lxe19f</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Purple with green magnetic polish dupe for this?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxe19f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1lxdref</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>When it’s your last mani out of a discontinued polish</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tsuhbz02bacf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1lxdp7q</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>In a pickle🥒</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxdp7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1lxdkx3</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>🍨 Painted Polish Mint Chip Madness 🍦 Instant mood booster!</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxdkx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1lxdksw</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Are you a collector or a painter?</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnkkhedv9acf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1lxcsie</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>My Attempt at Magnet Madness</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxcsie</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1lxckgi</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Reality check, please 😭 am I crazy or is the base color orange-brown on me?!</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxckgi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1lxc99e</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Life brand polish</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2xrxxln0acf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1lxby58</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Finally own choose life!</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/87ajex2iy9cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1lxbg6p</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxbg6p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1lxbfff</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Polish and Beauty Expo?</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lxbfff/polish_and_beauty_expo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1lxbf2g</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>First polish post!</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxbf2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1lxajnv</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Magnetic Techniques, Featuring High Roller</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5cmgr1dwo9cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1lxa5ko</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>I got my first solar polish and it‘s glorious</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxa5ko</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1lx9sjm</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>"Fish fear me. Women fear me. Police want me." (sound on)</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f6qsmt3qj9cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1lx9moo</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Essie Wicked is darker than expected</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx9moo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1lx9k50</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Low tech Magnetic Pearl Spinny Contraption</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6v4xk7v0i9cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1lx97qv</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Dupe for original Queen of Rot?</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx97qv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1lx8qt8</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lx8qt8/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1lx8p84</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Cosmic Polish Quicksilver + jelly polish over the top?</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lx8p84/cosmic_polish_quicksilver_jelly_polish_over_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1lx8fsl</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Waiting under a tree until it stops raining feat. Emily de molly Behind again 😀</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx8fsl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1lx86rj</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Idk why I waited so long to try this juicy flakie! 💚</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/houvus0989cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1lx83jo</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>New nail shape, who dis?</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx83jo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1lx7ymr</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>First Lurid Lacquer order 🤩🤩 thoughts?</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odhl341m69cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1lx7sap</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Flight of the Monarchs</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx7sap</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1lx75tp</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Cider made me do this combo ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx75tp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1lx5vyb</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>ILNP's Horseshoe Magnets</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lx5vyb/ilnps_horseshoe_magnets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1lx3y6m</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Mood Moo Deng Nails</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx3y6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1lx3gma</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Tragedy has struck</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx3gma</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1lx35rf</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>My low effort bead technique for those who don't have spinning contraptions!</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7vkkvyfuz7cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1lx2741</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Holo tips</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z8tu3moso7cf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1lxsj64</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Needing to find a colour</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxsj64</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1lxr2wk</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>The retention is retentioning</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxr2wk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1lxr2eo</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Nails for this week</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6u0xq1ncadcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1lxptlx</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Giving icy stare and metallic flair ❄️💅</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wm0h8oayccf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1lxpa9d</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Hot dog theme! Handmade by me!!</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgn2wnv7tccf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1lxozfe</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Design made for a wedding 😍</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9cun2oeqccf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1lxmc3n</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Are all gel polish magnetic?</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lxmc3n/are_all_gel_polish_magnetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1lxlhg9</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Bee mines 🐝</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgaprxm3wbcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1lxhm69</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Inky Chrome Freestyle 🩷🖤</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r9wu46bd2bcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1lxh62l</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>For Hello Kitty lovers, a design I made recently</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fl3yfwgazacf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1lxgw9t</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Summer Nails</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxgw9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1lxg8z6</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>I challenged myself to handpaint a Rumi nail set 😫 This art style has me in a chokehold</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xtp44pynsacf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1lxfd4e</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>July previous post got deleted</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ab4saxpdmacf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1lxc6pg</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Can i seal my press ons like gel x?</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lxc6pg/can_i_seal_my_press_ons_like_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1lxbsvl</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>What do you recommend I do on my nails? I'm about 15 years old?</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrodt4ijx9cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1lxb6qn</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Birthday set!</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxb6qn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1lx9q89</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Diseño floral!! 💐</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0x52nfa5j9cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1lx9m1z</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>I made them from home, do I add decoration?</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65tpyaahi9cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1lx8ldj</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Something fun for my clients vacation ✨💜</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wd8kxhn8b9cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1lx7lvr</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Cuteness overload... Trying a new shape</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lx7lvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1lx703k</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Beach nails</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2ea9ilbz8cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1lx6twv</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>DIY Press-On Nails Tutorial | How to Make Customized Press-On Nails at Home?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lx6twv/diy_presson_nails_tutorial_how_to_make_customized/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1lx5i6d</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Summer!!!</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lto7si3n8cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jul 13 08:11:13 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_13.xlsx
+++ b/data/collected_data/2025_07_13.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1337"/>
+  <dimension ref="A1:C1542"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23162,6 +23162,3491 @@
         </is>
       </c>
     </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1lyn9j6</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>My first attempt at hand painting a character on a nail.😊</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzf39p2lklcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1lymqbb</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Constantly getting halfway and wanting to give up 🙃</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/te4xtgcaelcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1lym8nm</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>I kinda hate these ngl</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lym8nm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1lylq37</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Classic pink ombré with a dash of flair</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbf4zutq2lcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1lylbey</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>I wish I didn’t do the gold….</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7a9b0w6aykcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1lykspg</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Me and My Client Got Hungry Mid-Session… So We Put It on Her Nails</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lykspg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1lyj8mv</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>What do you enjoy most about your day in the salon?</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ay9qhjzxckcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1lyik9n</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Crab Chrome Nails - at home job</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyik9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1lyihn4</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Chrome nails</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1xvr5lm5kcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1lyignh</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Cost question</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lyignh/cost_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1lyiah2</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Ballerina Love ❤️</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyiah2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1lyi1el</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>First post :&gt;</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wzt31nlb1kcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1lyajdx</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>I heard we’re doing butter yellow 🧈🌼</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyajdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1lya9mv</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>butterfly 𐀔 inspired</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rw6m75ii6icf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1ly7tkr</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Question about first manicure time</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ly7tkr/question_about_first_manicure_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1lyh1ci</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Pink Chrome! 💕</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j45hkjvurjcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1ly89ng</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Prr</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly89ng</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1ly98m2</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Gyaru inspired squares</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly98m2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1lyaftt</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>The Inspo pic and what art my nail tech did</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyaftt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1lyfffv</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>I get so much inspiration from Reddit nails</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9p08bws8djcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1lyfqpu</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Pink alien abduction nails</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6x4os7r1gjcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1lyhe2q</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Made some Powerpuff Girls aquarium press ons</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fk8iivn5vjcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1lyh9rt</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Dip powder on natural nails</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cx0ijfb1ujcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1lyh83z</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Tips to prevent robbery base from lifting?</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lyh83z/tips_to_prevent_robbery_base_from_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1lycuor</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>I’m ready to do my nails on my own.</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lycuor</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1lygkvd</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Your thoughts please?</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lygkvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1lygb6l</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Did my nails for CC Tour!!!!</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lygb6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1lyg58k</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>In a green mood 🪲</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyg58k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1lyg0gi</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>💛🍋🌼</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zz16067iijcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1lyfo85</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>No sun today, but these still look great in the shade!</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyfo85</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1lyfn0a</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Maybelline - blackened bronze</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyfn0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1lyfap8</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>💓💓💓</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0170up82cjcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1lyf6xs</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Is it ok to have nail lacquer on to go get a pedicure?</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lyf6xs/is_it_ok_to_have_nail_lacquer_on_to_go_get_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1lyepbj</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>What did they do to my nails??</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4j1c5b8t6jcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1lyegcf</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Green chrome 💚🧜🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyegcf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1ly4od4</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Is there a latex free peel off base?</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ly4od4/is_there_a_latex_free_peel_off_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1lyebap</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Best false nails to paint on with gel polish?</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lyebap/best_false_nails_to_paint_on_with_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1lye85q</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Baby nail clippers</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lye85q/baby_nail_clippers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1lye7i1</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>GTA/Rockstar Games nails at home</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lye7i1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1lye2be</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>I am not happy about the nail design I got and I want to change them already.</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovbwem7c1jcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1lydppw</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Please guess how long ago I did my nails?💅</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lydppw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1lydlo9</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>How can I save these?</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lydlo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1lydjzd</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>How are my reshaping skills? I am still very much a beginner.</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lydjzd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1lybv7b</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>💐</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45msj7z3jicf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1lybnq8</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>summer nails</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpzmm5ifhicf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1lyaub9</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Shape?</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyaub9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1lyaq5o</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Mushroom Manicure</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyaq5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1lya50y</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>First time!!</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lya50y/first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1lya4aw</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>July nails🪻</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jub9fqe5icf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1ly9x5y</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Simple Black French</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0masxyp3icf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1ly9pdn</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Russian mani with builder gel</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly9pdn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1ly9n0v</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Moo</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kaptpetn1icf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1ly9hgr</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>what are these white spots on the corner of my nails?</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly9hgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1ly9b4j</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Cateyes and MRI</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DMA8367skyB/?igsh=MXR1YmRuN3hiMnN0cQ==</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1ly9azx</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>polka dot party</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/032aubb3zhcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1ly8u2x</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>DIY Gel Nail Strips 💅</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/evrmentdvhcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1ly8sc7</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Two recent sets 💅</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly8sc7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1ly8ffl</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Holographic and mermaid chrome</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly8ffl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1ly8e13</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Yall it’s only just been a week   do my nails just grow fast?</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ck54bfx1shcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1ly8df5</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Thought I’d try something new, so green jelly it is 😊</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7e4fsckxrhcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1ly8526</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>fresh set! Picnic vibes and polka dots!</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly8526</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1ly80jo</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>blue manicure</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cfcnp9y7phcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1ly7zt3</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>First Time Doing French Tips at ho(m)e</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly7zt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1ly7qxb</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>i am so in love 💅🏾 press ons btw</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5h7sgug6nhcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1ly7lpj</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Nail artist killed this</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly7lpj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1ly7dc9</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Simple but i love it</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly7dc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1ly6t7q</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>What do you think of this combination?</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygauyz77ghcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1ly6ohk</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Cinderella dream nails</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yutecko5fhcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1ly6h03</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>New Glitter</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly6h03</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1ly64q4</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Decided To Try A New Color</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly64q4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1ly639v</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Chrome Watermelons</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0syejefvahcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1ly5nr8</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>So In Love With This Set</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8iz8pop7hcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1ly5l5d</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>recent nails ૮ ˶ᵔ ᵕ ᵔ˶ ა</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly5l5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1ly5euv</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Some sets I've done!</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/95rzf53p5hcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1ly569t</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Monopoly man</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly569t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1ly4u90</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>How should I manicure my nails?</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly4u90</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1ly489p</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>🤎🤎🤎</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly489p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1ly44td</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>on vacation and had to get my nails done</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xyncdwfzvgcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1ly41bh</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Fruit Salad!</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly41bh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1ly3h7s</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Break on only top layer?</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rv3q6eh6rgcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1ly3csj</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Shellac pros:</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ly3csj/shellac_pros/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1ly33qq</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>My summer nails - hubby was with me the first time</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/srfgi7qeogcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1ly2u5k</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Mix n Match Set for July 🌈</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly2u5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1ly2ix3</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Cat-eye shorties!</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bztmjpvyjgcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1ly2h92</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>I’m a fall girly just trying to get ideas for the fall</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yewgelenjgcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1lxzuq6</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Im a complete beginner and I need all the tips i can get.</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lxzuq6/im_a_complete_beginner_and_i_need_all_the_tips_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1lxy2to</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>how do you like this pink and yellow set?</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxy2to</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1lxuxnu</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>how do i even begin to heal them 😭</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34z5mm1rfecf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1lxun9g</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>When the drink was the inspo</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxun9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1ly24pc</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Nail rotted at the beach</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tb9zk4kzggcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1ly1x3u</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>First time practicing with Rubber</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ai70b6dbfgcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1ly1ryy</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>You guys!!!</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6j8h7j7egcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1ly1llk</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>My summer nails</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uj8d8unscgcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1ly1549</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>My first attempt at doing my own nails</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5l7vs869gcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1ly0kdj</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>loving this blue!</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly0kdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1ly0ftx</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Im in love with this color and shape</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ezbcj643gcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1ly066a</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Cute flower sticker</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly066a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1lxyc58</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>My Fourth of July nails</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7wfj4rpjfcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1lxxrvc</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>brittle and splotchy nails</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxxrvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1lxxl6s</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>July nails</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxxl6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1lyn4a5</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>an MRI tech has the opportunity to do the funniest thing</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9n8xumtilcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1lyjypr</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Cock a doodle doom dupe attempt</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/clixems3kkcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1lyijx5</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Opal nails</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyijx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1lyige3</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>Holo Taco Unicorn Skin Toppers</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lyige3/holo_taco_unicorn_skin_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1lyiaq9</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>Trying to get a good pic before the sun goes down haha</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyiaq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1lyi8ki</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Naked (nails) and afraid</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfpt8qwpujcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1lyhshs</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>What does this magnet do?</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2aebykgzyjcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1lyhj6n</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Lovely neutral yellow 🫖</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyhj6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1lygtof</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Not a fan of holo or metallic, but that’s all I’m seeing</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lygtof/not_a_fan_of_holo_or_metallic_but_thats_all_im/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1lygqln</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Natural nails</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lygqln</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1lygo3s</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>ILNP High Roller</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lygo3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1lyfr8l</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>Obsessed with this color!</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfrjjah6gjcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1lyfoqj</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>Second try of the Etsy magnetic 🧲 Green lovers unite 🍏</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k3wi8nwgfjcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1lyfnqw</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>BKL at the laundromat</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekx4nxo9fjcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1lyfl1m</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>Giving aura nails a try again!</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyfl1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1lyenjc</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Lucky and Bobon Jelly</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5egekxd6jcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1lyehff</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>Drown My Demons</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/60ejh7qw4jcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1lyeh7n</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>I don't have the right type of magnet, nor do I have magnetic nail polish, but an idea for my spinning sisters!</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2h26h1mt4jcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1lyedn9</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>Manhattan Cupcake Addict Dupe?</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lyedn9/manhattan_cupcake_addict_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1lyearq</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>Stella Chroma - Classic Red</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aiiat6qt2jcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1lye7lz</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>Baby nail clippers</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lye7lz/baby_nail_clippers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1lyd8cg</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Peeling polish</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lyd8cg/peeling_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1lycnko</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>Comparison request sassy sauce and Pfd</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lycnko/comparison_request_sassy_sauce_and_pfd/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1lyco9v</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>Sherbet Jelly</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyco9v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1lycdle</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>ISO Deep Toned Green Blue Duochrome</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ie1pepebnicf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1lyccq3</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>lurid lacquer</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyccq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1lyc70b</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Pink Pony Club 💖🐎</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyc70b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1lyc58z</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>A Witch’s Mana</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xg3k86h2licf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1lybtgn</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>After a few years of only doing basic, one color nails, I tried painting a ladybug design. I forgot how fun having nail designs was!</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqj25ugpiicf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1lybm86</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>Is anyone else….</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lybm86/is_anyone_else/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1lyb5qj</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>We all know Simone would approve</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjlnrq9ddicf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1lyasn1</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>{PR}Sassy Sauce Polish – Hanky Panky | HHC July 2025</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyasn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1lyak10</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>Ahhh. Comfort polish…</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0srlbjp8icf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1lyafcp</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>Glass bead effect with bar magnets!</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6owqu7tp7icf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1lya8l0</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>Showgirl ✨💅🏻✨</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s7szatva6icf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1ly9oui</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>Unknown (to me) uses for a nail stamper, but…how?</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7sd4asz12icf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1ly8kpj</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>Such shiftiness!</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly8kpj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1ly8224</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>New technique just dropped:</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b42j2yyjphcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1ly7xc1</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>Carina</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2wga4wejohcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1ly7maq</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>Lacquered up for Superman (and rip to this gorgeous shade)</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly7maq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1ly7gu4</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>Loving this Reflective Shimmer!</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x6achw32lhcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1ly7e4y</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>Help with swatch sticks please!</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ku4iltdckhcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1ly7cei</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>My first attempt at swirls with regular polish</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n86bcn26khcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1ly73a4</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>You all have made this my favorite time to be a laquerista.</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z8j59eh2ihcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>1ly6xzw</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>trans pride butterfly nails ✨</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly6xzw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>1ly6tlt</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>Starrily skittle</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly6tlt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>1ly6044</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>A not so unhinged glass bead method</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7yr37x28ahcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>1ly5y2t</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>First Gradient Attempt</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ly5y2t/first_gradient_attempt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>1ly4wai</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>Sour Apple Rings arrived just in time for 80s night. Wasn’t expecting this literal GLOW 🌟</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u33rsu7j1hcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>1ly4cvl</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>I had to jump on the crazy contraption trend!!</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/osnrpj6lxgcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>1ly3vbj</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquers - Kaleidoscope of Butterflies (PPU May 2025</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1yc9nwk5ugcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>1ly3rgt</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>What nail shape would suit me?</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly3rgt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" t="inlineStr">
+        <is>
+          <t>1ly3iqx</t>
+        </is>
+      </c>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>4ever Unsolved!</t>
+        </is>
+      </c>
+      <c r="C1490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly3iqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" t="inlineStr">
+        <is>
+          <t>1ly3iet</t>
+        </is>
+      </c>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>Is this greedy or a bad idea? I don't think so.</t>
+        </is>
+      </c>
+      <c r="C1491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ly3iet/is_this_greedy_or_a_bad_idea_i_dont_think_so/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" t="inlineStr">
+        <is>
+          <t>1ly3bvs</t>
+        </is>
+      </c>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>The commitment to the stunning backdrop never sleeps</t>
+        </is>
+      </c>
+      <c r="C1492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly3bvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1493">
+      <c r="A1493" t="inlineStr">
+        <is>
+          <t>1ly3598</t>
+        </is>
+      </c>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>Thermal polish broke in the middle of a mani</t>
+        </is>
+      </c>
+      <c r="C1493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2n1b91hqogcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" t="inlineStr">
+        <is>
+          <t>1ly34ni</t>
+        </is>
+      </c>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>This is hilarious</t>
+        </is>
+      </c>
+      <c r="C1494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly34ni</t>
+        </is>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" t="inlineStr">
+        <is>
+          <t>1ly1woy</t>
+        </is>
+      </c>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t>Holy Sparkles!</t>
+        </is>
+      </c>
+      <c r="C1495" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iqdjb4c8fgcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1496">
+      <c r="A1496" t="inlineStr">
+        <is>
+          <t>1ly1wou</t>
+        </is>
+      </c>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>Nothing about magnets, I’m afraid 😅</t>
+        </is>
+      </c>
+      <c r="C1496" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8fmc27c8fgcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" t="inlineStr">
+        <is>
+          <t>1ly1s38</t>
+        </is>
+      </c>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>UK: is anyone else looking to buy from Royla Lee’s new release and want to do a group buy?</t>
+        </is>
+      </c>
+      <c r="C1497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ly1s38/uk_is_anyone_else_looking_to_buy_from_royla_lees/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" t="inlineStr">
+        <is>
+          <t>1ly1lbn</t>
+        </is>
+      </c>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>Green attitude</t>
+        </is>
+      </c>
+      <c r="C1498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly1lbn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1499">
+      <c r="A1499" t="inlineStr">
+        <is>
+          <t>1ly19lh</t>
+        </is>
+      </c>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t>Just a Phase</t>
+        </is>
+      </c>
+      <c r="C1499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly19lh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1500">
+      <c r="A1500" t="inlineStr">
+        <is>
+          <t>1ly0c4o</t>
+        </is>
+      </c>
+      <c r="B1500" t="inlineStr">
+        <is>
+          <t>Leafy green ☺️🌿</t>
+        </is>
+      </c>
+      <c r="C1500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly0c4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1501">
+      <c r="A1501" t="inlineStr">
+        <is>
+          <t>1lxzuip</t>
+        </is>
+      </c>
+      <c r="B1501" t="inlineStr">
+        <is>
+          <t>My own (failed) attempt at the new magnet techique!</t>
+        </is>
+      </c>
+      <c r="C1501" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6s9lazmyxfcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1502">
+      <c r="A1502" t="inlineStr">
+        <is>
+          <t>1lxzqqs</t>
+        </is>
+      </c>
+      <c r="B1502" t="inlineStr">
+        <is>
+          <t>I need six strong women and a merry go round</t>
+        </is>
+      </c>
+      <c r="C1502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7i06oi7xfcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1503">
+      <c r="A1503" t="inlineStr">
+        <is>
+          <t>1lxzo6u</t>
+        </is>
+      </c>
+      <c r="B1503" t="inlineStr">
+        <is>
+          <t>Is anyone else disappointed with OPI’s collections lately?</t>
+        </is>
+      </c>
+      <c r="C1503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lxzo6u/is_anyone_else_disappointed_with_opis_collections/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1504">
+      <c r="A1504" t="inlineStr">
+        <is>
+          <t>1lxznek</t>
+        </is>
+      </c>
+      <c r="B1504" t="inlineStr">
+        <is>
+          <t>a little ghost inspo</t>
+        </is>
+      </c>
+      <c r="C1504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxznek</t>
+        </is>
+      </c>
+    </row>
+    <row r="1505">
+      <c r="A1505" t="inlineStr">
+        <is>
+          <t>1lxzmj6</t>
+        </is>
+      </c>
+      <c r="B1505" t="inlineStr">
+        <is>
+          <t>It's time for ✨️sparkle sadness✨️</t>
+        </is>
+      </c>
+      <c r="C1505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxzmj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1506">
+      <c r="A1506" t="inlineStr">
+        <is>
+          <t>1lxyff4</t>
+        </is>
+      </c>
+      <c r="B1506" t="inlineStr">
+        <is>
+          <t>Several questions about the nail polishes you use (the ones with metal particles in them).</t>
+        </is>
+      </c>
+      <c r="C1506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lxyff4/several_questions_about_the_nail_polishes_you_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1507">
+      <c r="A1507" t="inlineStr">
+        <is>
+          <t>1lxxoho</t>
+        </is>
+      </c>
+      <c r="B1507" t="inlineStr">
+        <is>
+          <t>May I suggest the humble box + cutout setup?</t>
+        </is>
+      </c>
+      <c r="C1507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lxxoho</t>
+        </is>
+      </c>
+    </row>
+    <row r="1508">
+      <c r="A1508" t="inlineStr">
+        <is>
+          <t>1lxri4t</t>
+        </is>
+      </c>
+      <c r="B1508" t="inlineStr">
+        <is>
+          <t>Anyone else loving Madam Glam gel polishes lately? 💅</t>
+        </is>
+      </c>
+      <c r="C1508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lxri4t/anyone_else_loving_madam_glam_gel_polishes_lately/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1509">
+      <c r="A1509" t="inlineStr">
+        <is>
+          <t>1lyn4gq</t>
+        </is>
+      </c>
+      <c r="B1509" t="inlineStr">
+        <is>
+          <t>My first attempt at hand painting a character on a nail.😊</t>
+        </is>
+      </c>
+      <c r="C1509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tr2wxawvilcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1510">
+      <c r="A1510" t="inlineStr">
+        <is>
+          <t>1lymk3j</t>
+        </is>
+      </c>
+      <c r="B1510" t="inlineStr">
+        <is>
+          <t>How much do you charge for sculpted nails with charms, 3D Flowers</t>
+        </is>
+      </c>
+      <c r="C1510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwjecwuaclcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1511">
+      <c r="A1511" t="inlineStr">
+        <is>
+          <t>1lymb36</t>
+        </is>
+      </c>
+      <c r="B1511" t="inlineStr">
+        <is>
+          <t>The Nail Company</t>
+        </is>
+      </c>
+      <c r="C1511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lymb36/the_nail_company/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1512">
+      <c r="A1512" t="inlineStr">
+        <is>
+          <t>1lyjken</t>
+        </is>
+      </c>
+      <c r="B1512" t="inlineStr">
+        <is>
+          <t>This is what I did for July 4th.</t>
+        </is>
+      </c>
+      <c r="C1512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lyjken/this_is_what_i_did_for_july_4th/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1513">
+      <c r="A1513" t="inlineStr">
+        <is>
+          <t>1lyks35</t>
+        </is>
+      </c>
+      <c r="B1513" t="inlineStr">
+        <is>
+          <t>Nail Session Got Us Hungry, So We Did a Tomato &amp; Egg Design for Fun</t>
+        </is>
+      </c>
+      <c r="C1513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyks35</t>
+        </is>
+      </c>
+    </row>
+    <row r="1514">
+      <c r="A1514" t="inlineStr">
+        <is>
+          <t>1lyjhqm</t>
+        </is>
+      </c>
+      <c r="B1514" t="inlineStr">
+        <is>
+          <t>July nails</t>
+        </is>
+      </c>
+      <c r="C1514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyjhqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1515">
+      <c r="A1515" t="inlineStr">
+        <is>
+          <t>1lyj1m5</t>
+        </is>
+      </c>
+      <c r="B1515" t="inlineStr">
+        <is>
+          <t>First attempt at doing my own nail art - I think I’ve got a new hobby</t>
+        </is>
+      </c>
+      <c r="C1515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyj1m5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1516">
+      <c r="A1516" t="inlineStr">
+        <is>
+          <t>1lyh5le</t>
+        </is>
+      </c>
+      <c r="B1516" t="inlineStr">
+        <is>
+          <t>Labubu fever 😂</t>
+        </is>
+      </c>
+      <c r="C1516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/suafnirysjcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1517">
+      <c r="A1517" t="inlineStr">
+        <is>
+          <t>1lyh3j9</t>
+        </is>
+      </c>
+      <c r="B1517" t="inlineStr">
+        <is>
+          <t>My Pride nails...because we do it in July in San Diego 😀</t>
+        </is>
+      </c>
+      <c r="C1517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyh3j9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1518">
+      <c r="A1518" t="inlineStr">
+        <is>
+          <t>1lyh1vf</t>
+        </is>
+      </c>
+      <c r="B1518" t="inlineStr">
+        <is>
+          <t>Natural nails: Dip powder with coffin shape and abstract design</t>
+        </is>
+      </c>
+      <c r="C1518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyh1vf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1519">
+      <c r="A1519" t="inlineStr">
+        <is>
+          <t>1lygjkz</t>
+        </is>
+      </c>
+      <c r="B1519" t="inlineStr">
+        <is>
+          <t>Chrome Tips</t>
+        </is>
+      </c>
+      <c r="C1519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lygjkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1520">
+      <c r="A1520" t="inlineStr">
+        <is>
+          <t>1lygi3x</t>
+        </is>
+      </c>
+      <c r="B1520" t="inlineStr">
+        <is>
+          <t>Made some PPG aquarium press ons</t>
+        </is>
+      </c>
+      <c r="C1520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zedio92umjcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1521">
+      <c r="A1521" t="inlineStr">
+        <is>
+          <t>1lyg6r3</t>
+        </is>
+      </c>
+      <c r="B1521" t="inlineStr">
+        <is>
+          <t>Pool season means Pool nails</t>
+        </is>
+      </c>
+      <c r="C1521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3n61ug1kjcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1522">
+      <c r="A1522" t="inlineStr">
+        <is>
+          <t>1lyfuom</t>
+        </is>
+      </c>
+      <c r="B1522" t="inlineStr">
+        <is>
+          <t>Pink alien abduction</t>
+        </is>
+      </c>
+      <c r="C1522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cqup2p92hjcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1523">
+      <c r="A1523" t="inlineStr">
+        <is>
+          <t>1lyf9lz</t>
+        </is>
+      </c>
+      <c r="B1523" t="inlineStr">
+        <is>
+          <t>Beach themed</t>
+        </is>
+      </c>
+      <c r="C1523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rz9sul3sbjcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1524">
+      <c r="A1524" t="inlineStr">
+        <is>
+          <t>1lyey70</t>
+        </is>
+      </c>
+      <c r="B1524" t="inlineStr">
+        <is>
+          <t>Trying different things</t>
+        </is>
+      </c>
+      <c r="C1524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyey70</t>
+        </is>
+      </c>
+    </row>
+    <row r="1525">
+      <c r="A1525" t="inlineStr">
+        <is>
+          <t>1lyeray</t>
+        </is>
+      </c>
+      <c r="B1525" t="inlineStr">
+        <is>
+          <t>Some ocean nails for my friend</t>
+        </is>
+      </c>
+      <c r="C1525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyeray</t>
+        </is>
+      </c>
+    </row>
+    <row r="1526">
+      <c r="A1526" t="inlineStr">
+        <is>
+          <t>1lyepx8</t>
+        </is>
+      </c>
+      <c r="B1526" t="inlineStr">
+        <is>
+          <t>First attempt of a chrome powder beetle</t>
+        </is>
+      </c>
+      <c r="C1526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqwl4dmy6jcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1527">
+      <c r="A1527" t="inlineStr">
+        <is>
+          <t>1lyefhk</t>
+        </is>
+      </c>
+      <c r="B1527" t="inlineStr">
+        <is>
+          <t>Pink power</t>
+        </is>
+      </c>
+      <c r="C1527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/en5a5tqf4jcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1528">
+      <c r="A1528" t="inlineStr">
+        <is>
+          <t>1lydwzo</t>
+        </is>
+      </c>
+      <c r="B1528" t="inlineStr">
+        <is>
+          <t>Work at home</t>
+        </is>
+      </c>
+      <c r="C1528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uev383h40jcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1529">
+      <c r="A1529" t="inlineStr">
+        <is>
+          <t>1lydf63</t>
+        </is>
+      </c>
+      <c r="B1529" t="inlineStr">
+        <is>
+          <t>Recent sets! For fun</t>
+        </is>
+      </c>
+      <c r="C1529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lydf63</t>
+        </is>
+      </c>
+    </row>
+    <row r="1530">
+      <c r="A1530" t="inlineStr">
+        <is>
+          <t>1lycmjx</t>
+        </is>
+      </c>
+      <c r="B1530" t="inlineStr">
+        <is>
+          <t>Did press ons for the first timee!!</t>
+        </is>
+      </c>
+      <c r="C1530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkysc02fpicf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1531">
+      <c r="A1531" t="inlineStr">
+        <is>
+          <t>1lyc8d0</t>
+        </is>
+      </c>
+      <c r="B1531" t="inlineStr">
+        <is>
+          <t>I want to hear opinions, how did they turn out for me?</t>
+        </is>
+      </c>
+      <c r="C1531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txnv07u4micf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1532">
+      <c r="A1532" t="inlineStr">
+        <is>
+          <t>1lyaobs</t>
+        </is>
+      </c>
+      <c r="B1532" t="inlineStr">
+        <is>
+          <t>Mushroom Nails</t>
+        </is>
+      </c>
+      <c r="C1532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lyaobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1533">
+      <c r="A1533" t="inlineStr">
+        <is>
+          <t>1ly9bou</t>
+        </is>
+      </c>
+      <c r="B1533" t="inlineStr">
+        <is>
+          <t>Nails for the summer are here 😍❤️</t>
+        </is>
+      </c>
+      <c r="C1533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ib0542k8zhcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1534">
+      <c r="A1534" t="inlineStr">
+        <is>
+          <t>1ly90b9</t>
+        </is>
+      </c>
+      <c r="B1534" t="inlineStr">
+        <is>
+          <t>Another one thank you 😊</t>
+        </is>
+      </c>
+      <c r="C1534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly90b9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1535">
+      <c r="A1535" t="inlineStr">
+        <is>
+          <t>1ly8ex0</t>
+        </is>
+      </c>
+      <c r="B1535" t="inlineStr">
+        <is>
+          <t>First time Y2K cheetah print</t>
+        </is>
+      </c>
+      <c r="C1535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly8ex0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1536">
+      <c r="A1536" t="inlineStr">
+        <is>
+          <t>1ly8a9s</t>
+        </is>
+      </c>
+      <c r="B1536" t="inlineStr">
+        <is>
+          <t>The most perfect nails i think ive ever done</t>
+        </is>
+      </c>
+      <c r="C1536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly8a9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1537">
+      <c r="A1537" t="inlineStr">
+        <is>
+          <t>1ly77jd</t>
+        </is>
+      </c>
+      <c r="B1537" t="inlineStr">
+        <is>
+          <t>Chrome powders - I found a solution to the messy, wasteful and inefficient system they come in 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1537" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lite222xihcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1538">
+      <c r="A1538" t="inlineStr">
+        <is>
+          <t>1ly6g43</t>
+        </is>
+      </c>
+      <c r="B1538" t="inlineStr">
+        <is>
+          <t>I'm starting, what figure do you recommend?</t>
+        </is>
+      </c>
+      <c r="C1538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyefrvlidhcf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1539">
+      <c r="A1539" t="inlineStr">
+        <is>
+          <t>1ly0ear</t>
+        </is>
+      </c>
+      <c r="B1539" t="inlineStr">
+        <is>
+          <t>Honest thoughts?</t>
+        </is>
+      </c>
+      <c r="C1539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2z9ht1v2gcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1540">
+      <c r="A1540" t="inlineStr">
+        <is>
+          <t>1ly08np</t>
+        </is>
+      </c>
+      <c r="B1540" t="inlineStr">
+        <is>
+          <t>my nails</t>
+        </is>
+      </c>
+      <c r="C1540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly08np</t>
+        </is>
+      </c>
+    </row>
+    <row r="1541">
+      <c r="A1541" t="inlineStr">
+        <is>
+          <t>1ly01uu</t>
+        </is>
+      </c>
+      <c r="B1541" t="inlineStr">
+        <is>
+          <t>This is my NailArt sampler. Would you make any of these designs? 🖤</t>
+        </is>
+      </c>
+      <c r="C1541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ly01uu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1542">
+      <c r="A1542" t="inlineStr">
+        <is>
+          <t>1lx4xr9</t>
+        </is>
+      </c>
+      <c r="B1542" t="inlineStr">
+        <is>
+          <t>Like my lucky nails, something good will happen to you today, it's no coincidence</t>
+        </is>
+      </c>
+      <c r="C1542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9lgru94i8cf1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>